<commit_message>
Style all data added
</commit_message>
<xml_diff>
--- a/Report1/DATA/Aneal_energies.xlsx
+++ b/Report1/DATA/Aneal_energies.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ciellie/PHD-Git/PHD/Report1/DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ciellie/PHD-Git/Report1/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Alpha Quartz</t>
   </si>
@@ -44,34 +44,37 @@
     <t>Cooling</t>
   </si>
   <si>
-    <t>4000-50</t>
-  </si>
-  <si>
-    <t>4000-100</t>
-  </si>
-  <si>
-    <t>4000-150</t>
-  </si>
-  <si>
-    <t>5000-50</t>
-  </si>
-  <si>
-    <t>5000-100</t>
-  </si>
-  <si>
-    <t>5000-150</t>
-  </si>
-  <si>
-    <t>6000-50</t>
-  </si>
-  <si>
-    <t>6000-100</t>
-  </si>
-  <si>
-    <t>6000-150</t>
-  </si>
-  <si>
     <t>Step</t>
+  </si>
+  <si>
+    <t>A-Alpha Quartz</t>
+  </si>
+  <si>
+    <t>B-4000-50</t>
+  </si>
+  <si>
+    <t>C-4000-100</t>
+  </si>
+  <si>
+    <t>D-4000-150</t>
+  </si>
+  <si>
+    <t>E-5000-50</t>
+  </si>
+  <si>
+    <t>F-5000-100</t>
+  </si>
+  <si>
+    <t>G-5000-150</t>
+  </si>
+  <si>
+    <t>H-6000-50</t>
+  </si>
+  <si>
+    <t>I-6000-100</t>
+  </si>
+  <si>
+    <t>J-6000-150</t>
   </si>
 </sst>
 </file>
@@ -388,13 +391,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -414,7 +419,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>-79498.141330059996</v>
@@ -434,7 +439,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>-79498.141330059996</v>
@@ -454,7 +459,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>-79498.141330059996</v>
@@ -474,7 +479,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>-79498.141330059996</v>
@@ -494,7 +499,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>-79498.141330059996</v>
@@ -514,7 +519,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>-79498.141330059996</v>
@@ -534,7 +539,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>-79498.141330059996</v>
@@ -554,7 +559,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>-79498.141330059996</v>
@@ -574,7 +579,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>-79498.141330059996</v>
@@ -594,7 +599,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>-79498.141330059996</v>

</xml_diff>